<commit_message>
debug form and code added form earlier project
</commit_message>
<xml_diff>
--- a/MissionControlModuleCs/doc/MissionControlModule - ROCket - WBS - sj2020 s5p1 - IC.xlsx
+++ b/MissionControlModuleCs/doc/MissionControlModule - ROCket - WBS - sj2020 s5p1 - IC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dick van Kalsbeek\Documents\_ROC archief niet in OneDrive\_Archief 2020 - 2021\VS2019\MissionControlModuleCs\MissionControlModuleCs\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{06E4DFE3-2C1F-42C7-B41E-18BCE80C1357}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EBC64F2-7124-42CF-8E21-8914BBD9EC20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,8 +19,8 @@
     <sheet name="version" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MCM!$A$4:$J$40</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">MCM!$A$1:$J$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MCM!$A$4:$J$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">MCM!$A$1:$J$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
   <si>
     <t>totaal</t>
   </si>
@@ -103,14 +103,6 @@
     <t>developer</t>
   </si>
   <si>
-    <t>duration
-(plan)</t>
-  </si>
-  <si>
-    <t>duration
-(do)</t>
-  </si>
-  <si>
     <t>reflection
 (check)</t>
   </si>
@@ -153,9 +145,6 @@
   </si>
   <si>
     <t>RS - compass - bearing</t>
-  </si>
-  <si>
-    <t>RS - acceleleration</t>
   </si>
   <si>
     <t>RS - temperature</t>
@@ -253,23 +242,51 @@
     <t>Stub</t>
   </si>
   <si>
-    <t>TX to GCM</t>
-  </si>
-  <si>
-    <t>RX from GCM</t>
-  </si>
-  <si>
     <t>MCM - basic design set up</t>
   </si>
   <si>
     <t>MCM - version control in GIT</t>
+  </si>
+  <si>
+    <t>duration
+(plan)
+min</t>
+  </si>
+  <si>
+    <t>duration
+(do)
+min</t>
+  </si>
+  <si>
+    <t>functions not the same as the real world</t>
+  </si>
+  <si>
+    <t>RS - acceleration</t>
+  </si>
+  <si>
+    <t>MCM - TX to GCM comm code and view (copy from earlier project)</t>
+  </si>
+  <si>
+    <t>MCM - RX from GCM comm code and view (copy from earlier project)</t>
+  </si>
+  <si>
+    <t>MCM - serial setup with Arduin/ESP32 (copy from earlier project)</t>
+  </si>
+  <si>
+    <t>problem with correct directory</t>
+  </si>
+  <si>
+    <t>handling now documented</t>
+  </si>
+  <si>
+    <t>MCM - debug window (copy from eralier project)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,6 +329,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -403,7 +426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -461,15 +484,24 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -753,11 +785,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
+      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -779,8 +811,8 @@
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="29"/>
       <c r="D1" s="3"/>
       <c r="E1" s="12"/>
       <c r="F1" s="17"/>
@@ -795,8 +827,8 @@
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="3"/>
       <c r="E2" s="12"/>
       <c r="F2" s="17"/>
@@ -809,10 +841,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="26"/>
+        <v>22</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
       <c r="D3" s="3"/>
       <c r="E3" s="12"/>
       <c r="F3" s="17"/>
@@ -831,7 +863,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>18</v>
@@ -840,71 +872,86 @@
         <v>19</v>
       </c>
       <c r="F4" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="5" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26">
+        <f>G43</f>
+        <v>630</v>
+      </c>
+      <c r="H5" s="26">
+        <f>H43</f>
+        <v>90</v>
+      </c>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+    </row>
+    <row r="6" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26">
+        <f>G5/60</f>
+        <v>10.5</v>
+      </c>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+    </row>
+    <row r="7" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>2</v>
@@ -912,10 +959,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>2</v>
@@ -923,10 +970,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>2</v>
@@ -934,10 +981,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>2</v>
@@ -945,10 +992,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
@@ -956,10 +1003,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>2</v>
@@ -967,10 +1014,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>2</v>
@@ -978,10 +1025,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>2</v>
@@ -989,267 +1036,337 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>11</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>13</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>14</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>15</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>16</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>17</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>18</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>19</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>20</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>21</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>12</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>13</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>14</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>15</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>16</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>17</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>18</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>19</v>
-      </c>
-      <c r="C24" s="1" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>22</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>20</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="D29" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>23</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>21</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="D30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>24</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>22</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>23</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="G31" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>25</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>24</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>25</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="D32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>26</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="C33" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G33" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>27</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>28</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>29</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>71</v>
+      <c r="C34" s="19" t="s">
+        <v>72</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="G34" s="1">
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" s="1">
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" s="1">
+        <v>30</v>
+      </c>
+      <c r="H36" s="1">
+        <v>90</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D40" s="1" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D42" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D41" s="2"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20">
-        <f>SUBTOTAL(9,G6:G40)</f>
-        <v>0</v>
-      </c>
-      <c r="H41" s="2">
-        <f>SUBTOTAL(9,H6:H40)</f>
-        <v>0</v>
-      </c>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20">
+        <f>SUBTOTAL(9,G8:G42)</f>
+        <v>630</v>
+      </c>
+      <c r="H43" s="2">
+        <f>SUBTOTAL(9,H8:H42)</f>
+        <v>90</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J40" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A4:J42" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
@@ -1272,34 +1389,34 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1497,13 +1614,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>25</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1511,10 +1628,10 @@
         <v>42286</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>